<commit_message>
AE-1500: initial setup with windows11 inventories
</commit_message>
<xml_diff>
--- a/tests/resources/workspace-001/windows11/02_analyzed/windows11-inventory_patched.xlsx
+++ b/tests/resources/workspace-001/windows11/02_analyzed/windows11-inventory_patched.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kklein/workspace/metaeffekt-workbench_gh/tests/resources/workspace-001/windows11/02_analyzed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A655C-CC09-D54A-95B4-52C036D87984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACAAC7-882C-984C-A8E1-5C103E2538E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="11300" windowWidth="32560" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3960" windowWidth="31220" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artifacts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Artifacts!$A$1:$K$65001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Artifacts!$A$1:$L$65001</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -64,9 +64,6 @@
     <t>10.0.26200.6901</t>
   </si>
   <si>
-    <t>cpe:/o:microsoft:windows_11, cpe:/o:microsoft:windows_11_23h2</t>
-  </si>
-  <si>
     <t>x64</t>
   </si>
   <si>
@@ -116,6 +113,24 @@
   </si>
   <si>
     <t>EOL Overwrite Cycle Query Version</t>
+  </si>
+  <si>
+    <t>Inapplicable CPE URIs</t>
+  </si>
+  <si>
+    <t>cpe:/o:microsoft:windows_11_25h2</t>
+  </si>
+  <si>
+    <t>cpe:/o:microsoft:windows_11_24h2</t>
+  </si>
+  <si>
+    <t>cpe:/o:microsoft:windows_11_23h2</t>
+  </si>
+  <si>
+    <t>cpe:/o:microsoft:windows_11</t>
+  </si>
+  <si>
+    <t>cpe:/o:microsoft:windows_11 is considered a outdated for this version of windows.</t>
   </si>
 </sst>
 </file>
@@ -501,16 +516,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="63.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,28 +552,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -556,93 +587,111 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>28</v>
       </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K65001" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L65001" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>